<commit_message>
All sceanri implementation done
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -38,13 +38,13 @@
     <t>Kids Premium T-Shirts</t>
   </si>
   <si>
-    <t>9-10 years</t>
+    <t>9-10 Years</t>
   </si>
   <si>
     <t>Black</t>
   </si>
   <si>
-    <t>5-6 years</t>
+    <t>5-6 Years</t>
   </si>
   <si>
     <t>White</t>

</xml_diff>